<commit_message>
[FIX] updating dougs name, minor xls formatting
</commit_message>
<xml_diff>
--- a/images/schedule.xlsx
+++ b/images/schedule.xlsx
@@ -53,7 +53,7 @@
     <t xml:space="preserve">The Brain Imaging Data Structure PET extension (Dr Melanie Ganz)</t>
   </si>
   <si>
-    <t xml:space="preserve">An overview of PetSurfer (Dr Douglas Greve)</t>
+    <t xml:space="preserve">An overview of PetSurfer (Dr Douglas N. Greve)</t>
   </si>
   <si>
     <t xml:space="preserve">Unconference / Projects Presentation</t>
@@ -137,16 +137,16 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF373737"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF373737"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -284,7 +284,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -293,7 +293,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -309,7 +309,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -321,10 +321,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -345,7 +341,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -357,7 +353,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -381,7 +377,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -397,11 +393,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -413,7 +409,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -501,7 +497,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -579,14 +575,14 @@
       <c r="I5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="n">
+      <c r="A6" s="6" t="n">
         <v>1000</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="8"/>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="6" t="n">
         <v>400</v>
       </c>
       <c r="F6" s="0"/>
@@ -595,12 +591,12 @@
       <c r="I6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="n">
+      <c r="A7" s="6" t="n">
         <v>1030</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="6" t="n">
         <v>430</v>
       </c>
       <c r="F7" s="0"/>
@@ -609,14 +605,14 @@
       <c r="I7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="n">
+      <c r="A8" s="6" t="n">
         <v>1100</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="9" t="n">
+      <c r="D8" s="6" t="n">
         <v>500</v>
       </c>
       <c r="F8" s="0"/>
@@ -625,12 +621,12 @@
       <c r="I8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="n">
+      <c r="A9" s="6" t="n">
         <v>1130</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="9" t="n">
+      <c r="D9" s="6" t="n">
         <v>530</v>
       </c>
       <c r="F9" s="0"/>
@@ -639,12 +635,12 @@
       <c r="I9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="n">
+      <c r="A10" s="6" t="n">
         <v>1200</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="9" t="n">
+      <c r="D10" s="6" t="n">
         <v>600</v>
       </c>
       <c r="F10" s="0"/>
@@ -653,12 +649,12 @@
       <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="n">
+      <c r="A11" s="6" t="n">
         <v>1230</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="9" t="n">
+      <c r="D11" s="6" t="n">
         <v>630</v>
       </c>
       <c r="F11" s="0"/>
@@ -667,12 +663,12 @@
       <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="n">
+      <c r="A12" s="6" t="n">
         <v>1300</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="9" t="n">
+      <c r="D12" s="6" t="n">
         <v>700</v>
       </c>
       <c r="F12" s="0"/>
@@ -681,12 +677,12 @@
       <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="n">
+      <c r="A13" s="6" t="n">
         <v>1330</v>
       </c>
-      <c r="B13" s="11"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="9" t="n">
+      <c r="D13" s="6" t="n">
         <v>730</v>
       </c>
       <c r="F13" s="0"/>
@@ -695,12 +691,12 @@
       <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="n">
+      <c r="A14" s="6" t="n">
         <v>1400</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="9" t="n">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="6" t="n">
         <v>800</v>
       </c>
       <c r="F14" s="0"/>
@@ -709,14 +705,14 @@
       <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="n">
+      <c r="A15" s="6" t="n">
         <v>1430</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="10"/>
+      <c r="C15" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="9" t="n">
+      <c r="D15" s="6" t="n">
         <v>830</v>
       </c>
       <c r="F15" s="0"/>
@@ -725,14 +721,14 @@
       <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="n">
+      <c r="A16" s="13" t="n">
         <v>1500</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16" t="n">
+      <c r="C16" s="14"/>
+      <c r="D16" s="15" t="n">
         <v>900</v>
       </c>
       <c r="F16" s="0"/>
@@ -741,14 +737,14 @@
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="n">
+      <c r="A17" s="16" t="n">
         <v>1530</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19" t="n">
+      <c r="C17" s="17"/>
+      <c r="D17" s="18" t="n">
         <v>930</v>
       </c>
       <c r="F17" s="0"/>
@@ -757,14 +753,14 @@
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="n">
+      <c r="A18" s="6" t="n">
         <v>1600</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="9" t="n">
+      <c r="C18" s="19"/>
+      <c r="D18" s="6" t="n">
         <v>1000</v>
       </c>
       <c r="F18" s="0"/>
@@ -773,12 +769,12 @@
       <c r="I18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="n">
+      <c r="A19" s="6" t="n">
         <v>1630</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="9" t="n">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="6" t="n">
         <v>1030</v>
       </c>
       <c r="F19" s="0"/>
@@ -787,14 +783,14 @@
       <c r="I19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="n">
+      <c r="A20" s="6" t="n">
         <v>1700</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="9" t="n">
+      <c r="D20" s="6" t="n">
         <v>1100</v>
       </c>
       <c r="F20" s="0"/>
@@ -803,14 +799,14 @@
       <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="n">
+      <c r="A21" s="6" t="n">
         <v>1730</v>
       </c>
       <c r="B21" s="8"/>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="9" t="n">
+      <c r="D21" s="6" t="n">
         <v>1130</v>
       </c>
       <c r="F21" s="0"/>
@@ -819,14 +815,14 @@
       <c r="I21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="n">
+      <c r="A22" s="6" t="n">
         <v>1800</v>
       </c>
       <c r="B22" s="8"/>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="9" t="n">
+      <c r="D22" s="6" t="n">
         <v>1200</v>
       </c>
       <c r="F22" s="0"/>
@@ -835,12 +831,12 @@
       <c r="I22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="n">
+      <c r="A23" s="6" t="n">
         <v>1830</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="9" t="n">
+      <c r="C23" s="23"/>
+      <c r="D23" s="6" t="n">
         <v>1230</v>
       </c>
       <c r="F23" s="0"/>
@@ -849,14 +845,14 @@
       <c r="I23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="n">
+      <c r="A24" s="6" t="n">
         <v>1900</v>
       </c>
       <c r="B24" s="8"/>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="9" t="n">
+      <c r="D24" s="6" t="n">
         <v>1300</v>
       </c>
       <c r="F24" s="0"/>
@@ -865,12 +861,12 @@
       <c r="I24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="n">
+      <c r="A25" s="6" t="n">
         <v>1930</v>
       </c>
       <c r="B25" s="8"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="9" t="n">
+      <c r="C25" s="24"/>
+      <c r="D25" s="6" t="n">
         <v>1330</v>
       </c>
       <c r="F25" s="0"/>
@@ -879,12 +875,12 @@
       <c r="I25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="n">
+      <c r="A26" s="6" t="n">
         <v>2000</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="9" t="n">
+      <c r="C26" s="24"/>
+      <c r="D26" s="6" t="n">
         <v>1400</v>
       </c>
       <c r="F26" s="0"/>
@@ -893,12 +889,12 @@
       <c r="I26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="n">
+      <c r="A27" s="6" t="n">
         <v>2030</v>
       </c>
       <c r="B27" s="8"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="9" t="n">
+      <c r="C27" s="24"/>
+      <c r="D27" s="6" t="n">
         <v>1430</v>
       </c>
       <c r="F27" s="0"/>
@@ -907,12 +903,12 @@
       <c r="I27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="n">
+      <c r="A28" s="6" t="n">
         <v>2100</v>
       </c>
       <c r="B28" s="8"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="9" t="n">
+      <c r="C28" s="24"/>
+      <c r="D28" s="6" t="n">
         <v>1500</v>
       </c>
       <c r="F28" s="0"/>
@@ -921,12 +917,12 @@
       <c r="I28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="26" t="n">
+      <c r="A29" s="25" t="n">
         <v>2130</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26" t="n">
+      <c r="B29" s="11"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="25" t="n">
         <v>1530</v>
       </c>
       <c r="F29" s="0"/>
@@ -946,7 +942,7 @@
       <c r="A32" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="5" t="s">
@@ -960,7 +956,7 @@
       <c r="A33" s="6" t="n">
         <v>900</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C33" s="8"/>
@@ -972,269 +968,269 @@
       <c r="A34" s="6" t="n">
         <v>930</v>
       </c>
-      <c r="B34" s="27"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="8"/>
       <c r="D34" s="6" t="n">
         <v>330</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="n">
+      <c r="A35" s="6" t="n">
         <v>1000</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C35" s="8"/>
-      <c r="D35" s="9" t="n">
+      <c r="D35" s="6" t="n">
         <v>400</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="n">
+      <c r="A36" s="6" t="n">
         <v>1030</v>
       </c>
-      <c r="B36" s="27"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="9" t="n">
+      <c r="D36" s="6" t="n">
         <v>430</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="n">
+      <c r="A37" s="6" t="n">
         <v>1100</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C37" s="8"/>
-      <c r="D37" s="9" t="n">
+      <c r="D37" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9" t="n">
+      <c r="A38" s="6" t="n">
         <v>1130</v>
       </c>
-      <c r="B38" s="11"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="9" t="n">
+      <c r="D38" s="6" t="n">
         <v>530</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="n">
+      <c r="A39" s="6" t="n">
         <v>1200</v>
       </c>
-      <c r="B39" s="11"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="9" t="n">
+      <c r="D39" s="6" t="n">
         <v>600</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="9" t="n">
+      <c r="A40" s="6" t="n">
         <v>1230</v>
       </c>
-      <c r="B40" s="11"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="9" t="n">
+      <c r="D40" s="6" t="n">
         <v>630</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="n">
+      <c r="A41" s="6" t="n">
         <v>1300</v>
       </c>
-      <c r="B41" s="11"/>
+      <c r="B41" s="10"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="9" t="n">
+      <c r="D41" s="6" t="n">
         <v>700</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9" t="n">
+      <c r="A42" s="6" t="n">
         <v>1330</v>
       </c>
-      <c r="B42" s="11"/>
+      <c r="B42" s="10"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="9" t="n">
+      <c r="D42" s="6" t="n">
         <v>730</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="9" t="n">
+      <c r="A43" s="6" t="n">
         <v>1400</v>
       </c>
-      <c r="B43" s="11"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="9" t="n">
+      <c r="D43" s="6" t="n">
         <v>800</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9" t="n">
+      <c r="A44" s="6" t="n">
         <v>1430</v>
       </c>
-      <c r="B44" s="11"/>
+      <c r="B44" s="10"/>
       <c r="C44" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="9" t="n">
+      <c r="D44" s="6" t="n">
         <v>830</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="14" t="n">
+      <c r="A45" s="13" t="n">
         <v>1500</v>
       </c>
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="16" t="n">
+      <c r="C45" s="27"/>
+      <c r="D45" s="15" t="n">
         <v>900</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="17" t="n">
+      <c r="A46" s="16" t="n">
         <v>1530</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="29"/>
-      <c r="D46" s="19" t="n">
+      <c r="C46" s="28"/>
+      <c r="D46" s="18" t="n">
         <v>930</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="9" t="n">
+      <c r="A47" s="6" t="n">
         <v>1600</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="20"/>
-      <c r="D47" s="9" t="n">
+      <c r="C47" s="19"/>
+      <c r="D47" s="6" t="n">
         <v>1000</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9" t="n">
+      <c r="A48" s="6" t="n">
         <v>1630</v>
       </c>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="9" t="n">
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="6" t="n">
         <v>1030</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="9" t="n">
+      <c r="A49" s="6" t="n">
         <v>1700</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="30" t="s">
+      <c r="B49" s="20"/>
+      <c r="C49" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D49" s="9" t="n">
+      <c r="D49" s="6" t="n">
         <v>1100</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="9" t="n">
+      <c r="A50" s="6" t="n">
         <v>1730</v>
       </c>
       <c r="B50" s="8"/>
-      <c r="C50" s="31" t="s">
+      <c r="C50" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D50" s="9" t="n">
+      <c r="D50" s="6" t="n">
         <v>1130</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9" t="n">
+      <c r="A51" s="6" t="n">
         <v>1800</v>
       </c>
       <c r="B51" s="8"/>
-      <c r="C51" s="32" t="s">
+      <c r="C51" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="9" t="n">
+      <c r="D51" s="6" t="n">
         <v>1200</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9" t="n">
+      <c r="A52" s="6" t="n">
         <v>1830</v>
       </c>
       <c r="B52" s="8"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="9" t="n">
+      <c r="C52" s="31"/>
+      <c r="D52" s="6" t="n">
         <v>1230</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9" t="n">
+      <c r="A53" s="6" t="n">
         <v>1900</v>
       </c>
       <c r="B53" s="8"/>
-      <c r="C53" s="33" t="s">
+      <c r="C53" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="D53" s="9" t="n">
+      <c r="D53" s="6" t="n">
         <v>1300</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9" t="n">
+      <c r="A54" s="6" t="n">
         <v>1930</v>
       </c>
       <c r="B54" s="8"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="9" t="n">
+      <c r="C54" s="32"/>
+      <c r="D54" s="6" t="n">
         <v>1330</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="n">
+      <c r="A55" s="6" t="n">
         <v>2000</v>
       </c>
       <c r="B55" s="8"/>
-      <c r="C55" s="33"/>
-      <c r="D55" s="9" t="n">
+      <c r="C55" s="32"/>
+      <c r="D55" s="6" t="n">
         <v>1400</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="9" t="n">
+      <c r="A56" s="6" t="n">
         <v>2030</v>
       </c>
       <c r="B56" s="8"/>
-      <c r="C56" s="33"/>
-      <c r="D56" s="9" t="n">
+      <c r="C56" s="32"/>
+      <c r="D56" s="6" t="n">
         <v>1430</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9" t="n">
+      <c r="A57" s="6" t="n">
         <v>2100</v>
       </c>
       <c r="B57" s="8"/>
-      <c r="C57" s="33"/>
-      <c r="D57" s="9" t="n">
+      <c r="C57" s="32"/>
+      <c r="D57" s="6" t="n">
         <v>1500</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="n">
+      <c r="A58" s="6" t="n">
         <v>2130</v>
       </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="26" t="n">
+      <c r="B58" s="11"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="25" t="n">
         <v>1530</v>
       </c>
     </row>

</xml_diff>